<commit_message>
feat: Complete React CPL Auction app with Supabase integration
- Convert Streamlit app to modern React application
- Add Supabase database integration for persistent data
- Implement CPL auction requirements with category budgets
- Add role-based auction phases (Batsmen  Bowlers  All-rounders  Wicket Keepers)
- Include timer system for exciting auction experience
- Add comprehensive Excel export functionality
- Implement mobile-responsive design with animations
- Add reset functionality for testing
- Include deployment configuration for Vercel
</commit_message>
<xml_diff>
--- a/assets/Cpl_data.xlsx
+++ b/assets/Cpl_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOOD\CODE\cplbidding\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="Teams" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>TeamID</t>
   </si>
@@ -223,15 +223,6 @@
   </si>
   <si>
     <t>spartans.jpg</t>
-  </si>
-  <si>
-    <t>warriors.jpg</t>
-  </si>
-  <si>
-    <t>T09</t>
-  </si>
-  <si>
-    <t>Silver Titans</t>
   </si>
 </sst>
 </file>
@@ -558,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,17 +661,6 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" t="s">
-        <v>66</v>
-      </c>
-    </row>
   </sheetData>
   <sortState ref="B2:B16">
     <sortCondition ref="B2"/>
@@ -693,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>